<commit_message>
Update System review status - Service Module.xlsx
</commit_message>
<xml_diff>
--- a/Workshop & Service Module/System review status - Service Module.xlsx
+++ b/Workshop & Service Module/System review status - Service Module.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\NexusProduct\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\NexusProduct\Documents\Workshop &amp; Service Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>No.</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>If OWN VEHICLE selected, then system should not SAVE if we enter OTHER VEHICLE number</t>
+  </si>
+  <si>
+    <t>Service Entry photo save path</t>
+  </si>
+  <si>
+    <t>Photos to be saved in folder and URL to be kept in DB</t>
   </si>
 </sst>
 </file>
@@ -149,28 +155,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -471,7 +456,7 @@
   <dimension ref="B2:G126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -542,16 +527,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
         <f t="shared" ref="B5:B68" si="0">B4+1</f>
         <v>3</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="6"/>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="6">
+        <v>43925</v>
+      </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
@@ -1797,13 +1790,13 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="G3:G126">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>